<commit_message>
Corrected codebook variable def
Changed from HC_distance to HC_time
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11210"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4963127-92F0-0841-87AC-4B2D2B0728A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD4884C-75B3-A54D-954A-A39C8055350B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10100" yWindow="500" windowWidth="20780" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10100" yWindow="500" windowWidth="20780" windowHeight="20200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>Height</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>identified gender (male/female/other)</t>
-  </si>
-  <si>
-    <t>HC_distance</t>
   </si>
   <si>
     <t>travel time to nearest healthcare facility (in minutes)</t>
@@ -433,7 +430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -453,10 +450,10 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -473,7 +470,7 @@
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -490,7 +487,7 @@
         <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -507,7 +504,7 @@
         <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -524,7 +521,7 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -541,7 +538,7 @@
         <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -558,7 +555,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -575,7 +572,7 @@
         <v>50</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -592,7 +589,7 @@
         <v>65</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -609,7 +606,7 @@
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -626,7 +623,7 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -640,7 +637,7 @@
         <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -657,7 +654,7 @@
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -674,7 +671,7 @@
         <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -691,7 +688,7 @@
         <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -703,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -760,10 +757,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
@@ -771,13 +768,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
         <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing if push works
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11210"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2C5468-D8F1-B744-97AD-BCE0B2489F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC171E9-3A6C-7543-AE66-9AF740ED5698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10100" yWindow="500" windowWidth="20780" windowHeight="20200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10100" yWindow="780" windowWidth="20780" windowHeight="19680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>Height</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>refused</t>
-  </si>
-  <si>
-    <t>numeric value &gt;0 or -999</t>
   </si>
 </sst>
 </file>
@@ -704,7 +701,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -766,7 +763,7 @@
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>